<commit_message>
Updated User Interface File
</commit_message>
<xml_diff>
--- a/Optimal_Decarbonisation_User_Interface.xlsx
+++ b/Optimal_Decarbonisation_User_Interface.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\OneDrive - University of Nottingham Malaysia\The University of Nottingham\BC COP26 Trilateral Research Initiative\BCCOP26TrilateralProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10682CAA-578B-45FA-9DE9-71DEA9C8032E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FE383E3-7985-4343-A572-0DB54E054469}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,15 +39,9 @@
     <t>LB</t>
   </si>
   <si>
-    <t>Lower bound for energy availability for each plant</t>
-  </si>
-  <si>
     <t>UB</t>
   </si>
   <si>
-    <t>Upper bound for energy availability for each plant</t>
-  </si>
-  <si>
     <t>CI</t>
   </si>
   <si>
@@ -409,6 +403,12 @@
   </si>
   <si>
     <t>TABLE 3: NET PARAMETERS</t>
+  </si>
+  <si>
+    <t>Lower bound for energy output for each plant</t>
+  </si>
+  <si>
+    <t>Upper bound for energy output for each plant</t>
   </si>
 </sst>
 </file>
@@ -574,7 +574,6 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -587,6 +586,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -923,7 +923,7 @@
   <dimension ref="A1:I67"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="B6" sqref="B6:D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -932,11 +932,11 @@
     <col min="2" max="2" width="20.85546875" style="1" customWidth="1"/>
     <col min="3" max="3" width="21.42578125" style="1" customWidth="1"/>
     <col min="4" max="9" width="19.85546875" style="1" customWidth="1"/>
-    <col min="10" max="30" width="9.140625" style="1" customWidth="1"/>
-    <col min="31" max="16384" width="9.140625" style="1"/>
+    <col min="10" max="34" width="9.140625" style="1" customWidth="1"/>
+    <col min="35" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="13" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="12" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
@@ -949,12 +949,12 @@
       <c r="H1" s="18"/>
       <c r="I1" s="18"/>
     </row>
-    <row r="2" spans="1:9" s="13" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" s="12" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" s="13" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" s="12" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -964,228 +964,228 @@
       <c r="C3" s="16"/>
       <c r="D3" s="17"/>
     </row>
-    <row r="4" spans="1:9" s="13" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" s="12" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>5</v>
+        <v>127</v>
       </c>
       <c r="C4" s="16"/>
       <c r="D4" s="17"/>
     </row>
-    <row r="5" spans="1:9" s="13" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" s="12" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>7</v>
+        <v>128</v>
       </c>
       <c r="C5" s="16"/>
       <c r="D5" s="17"/>
     </row>
-    <row r="6" spans="1:9" s="13" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" s="12" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C6" s="16"/>
       <c r="D6" s="17"/>
     </row>
-    <row r="7" spans="1:9" s="13" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" s="12" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C7" s="16"/>
       <c r="D7" s="17"/>
     </row>
-    <row r="8" spans="1:9" s="13" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" s="12" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C8" s="16"/>
       <c r="D8" s="17"/>
     </row>
-    <row r="9" spans="1:9" s="13" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" s="12" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C9" s="16"/>
       <c r="D9" s="17"/>
     </row>
-    <row r="10" spans="1:9" s="13" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" s="12" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C10" s="16"/>
       <c r="D10" s="17"/>
     </row>
-    <row r="11" spans="1:9" s="13" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" s="12" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C11" s="16"/>
       <c r="D11" s="17"/>
     </row>
-    <row r="12" spans="1:9" s="13" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" s="12" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C12" s="16"/>
       <c r="D12" s="17"/>
     </row>
-    <row r="13" spans="1:9" s="13" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" s="12" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C13" s="16"/>
       <c r="D13" s="17"/>
     </row>
-    <row r="14" spans="1:9" s="13" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="14"/>
-    </row>
-    <row r="15" spans="1:9" s="13" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="14" t="s">
+    <row r="14" spans="1:9" s="12" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="13"/>
+    </row>
+    <row r="15" spans="1:9" s="12" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" s="12" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" s="12" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:9" s="13" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="8" t="s">
+    <row r="18" spans="1:3" s="12" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="8" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:3" s="13" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="8" t="s">
+    <row r="19" spans="1:3" s="12" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="8" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:3" s="13" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" s="13" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="8" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" s="13" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" s="12" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5"/>
       <c r="B20" s="18" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C20" s="18"/>
     </row>
-    <row r="21" spans="1:3" s="13" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" s="12" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="7"/>
       <c r="B21" s="18" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C21" s="18"/>
     </row>
-    <row r="22" spans="1:3" s="13" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" s="12" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22" s="18"/>
+    </row>
+    <row r="23" spans="1:3" s="12" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:3" s="12" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" s="12" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="C22" s="18"/>
-    </row>
-    <row r="23" spans="1:3" s="13" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:3" s="13" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="8" t="s">
+      <c r="B25" s="7" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="25" spans="1:3" s="13" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="13" t="s">
+    <row r="26" spans="1:3" s="12" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="B25" s="7" t="s">
+      <c r="B26" s="7" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="26" spans="1:3" s="13" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="13" t="s">
+    <row r="27" spans="1:3" s="12" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="B26" s="7" t="s">
+      <c r="B27" s="7" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="27" spans="1:3" s="13" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="13" t="s">
+    <row r="28" spans="1:3" s="12" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B28" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B27" s="7" t="s">
+    </row>
+    <row r="29" spans="1:3" s="12" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:3" s="12" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="18" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" s="13" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="B28" s="7" t="s">
+      <c r="B30" s="18"/>
+    </row>
+    <row r="31" spans="1:3" s="12" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="12" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" s="13" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:3" s="13" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="18" t="s">
+      <c r="B31" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="B30" s="18"/>
-    </row>
-    <row r="31" spans="1:3" s="13" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="13" t="s">
+    </row>
+    <row r="32" spans="1:3" s="12" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="B31" s="8" t="s">
+      <c r="B32" s="8" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="32" spans="1:3" s="13" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="13" t="s">
+    <row r="33" spans="1:9" s="12" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="B32" s="8" t="s">
+      <c r="B33" s="7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" s="12" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="35" spans="1:9" s="12" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="19" t="s">
         <v>44</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" s="13" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="B33" s="7" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" s="13" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="35" spans="1:9" s="13" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="19" t="s">
-        <v>46</v>
       </c>
       <c r="B35" s="18"/>
       <c r="C35" s="18"/>
@@ -1196,62 +1196,62 @@
       <c r="H35" s="18"/>
       <c r="I35" s="18"/>
     </row>
-    <row r="36" spans="1:9" s="13" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" s="12" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D36" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C36" s="5" t="s">
+      <c r="E36" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="D36" s="5" t="s">
+      <c r="F36" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="E36" s="5" t="s">
+      <c r="G36" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="F36" s="5" t="s">
+      <c r="H36" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="G36" s="5" t="s">
+      <c r="I36" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="H36" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="I36" s="5" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" s="13" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:9" s="12" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B37" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="F37" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="C37" s="6" t="s">
+      <c r="G37" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="D37" s="6" t="s">
+      <c r="H37" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="E37" s="6" t="s">
+      <c r="I37" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="F37" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="G37" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="H37" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="I37" s="6" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" s="13" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:9" s="12" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>4</v>
       </c>
@@ -1280,9 +1280,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:9" s="13" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" s="12" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B39" s="6">
         <v>40</v>
@@ -1309,9 +1309,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="40" spans="1:9" s="13" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" s="12" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B40" s="6">
         <v>0</v>
@@ -1338,9 +1338,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:9" s="13" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" s="12" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B41" s="6">
         <v>0</v>
@@ -1367,9 +1367,9 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="42" spans="1:9" s="13" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" s="12" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B42" s="6">
         <v>0</v>
@@ -1396,9 +1396,9 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="43" spans="1:9" s="13" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" s="12" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B43" s="6">
         <v>0</v>
@@ -1425,9 +1425,9 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="44" spans="1:9" s="13" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" s="12" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B44" s="6">
         <v>0</v>
@@ -1454,9 +1454,9 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="45" spans="1:9" s="13" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" s="12" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B45" s="6">
         <v>155</v>
@@ -1483,9 +1483,9 @@
         <v>51</v>
       </c>
     </row>
-    <row r="46" spans="1:9" s="13" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" s="12" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B46" s="6">
         <v>0</v>
@@ -1512,9 +1512,9 @@
         <v>82</v>
       </c>
     </row>
-    <row r="47" spans="1:9" s="13" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" s="12" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B47" s="6">
         <v>0</v>
@@ -1542,217 +1542,217 @@
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A48" s="13"/>
-      <c r="B48" s="13"/>
-      <c r="C48" s="13"/>
-      <c r="D48" s="13"/>
+      <c r="A48" s="12"/>
+      <c r="B48" s="12"/>
+      <c r="C48" s="12"/>
+      <c r="D48" s="12"/>
     </row>
     <row r="49" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="13" t="s">
+      <c r="A49" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="B49" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C49" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="D49" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="E49" s="12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="B50" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="C50" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="D50" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="E50" s="12" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="B49" s="13" t="s">
+      <c r="B51" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C51" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="D51" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="E51" s="12" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="B52" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="C52" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="D52" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="E52" s="12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="12"/>
+      <c r="B53" s="12"/>
+      <c r="C53" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="C49" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="D49" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="E49" s="13" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="B50" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="C50" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="D50" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="E50" s="13" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="B51" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="C51" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="D51" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="E51" s="13" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="B52" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="C52" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="D52" s="13" t="s">
+      <c r="D53" s="12"/>
+      <c r="E53" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="E52" s="13" t="s">
+    </row>
+    <row r="54" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="12"/>
+      <c r="B54" s="12"/>
+      <c r="C54" s="12" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="13"/>
-      <c r="B53" s="13"/>
-      <c r="C53" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="D53" s="13"/>
-      <c r="E53" s="13" t="s">
+      <c r="D54" s="12"/>
+      <c r="E54" s="12" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="54" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="13"/>
-      <c r="B54" s="13"/>
-      <c r="C54" s="13" t="s">
+    <row r="55" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="12"/>
+      <c r="B55" s="12"/>
+      <c r="C55" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="D54" s="13"/>
-      <c r="E54" s="13" t="s">
+      <c r="D55" s="12"/>
+      <c r="E55" s="12" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="55" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="13"/>
-      <c r="B55" s="13"/>
-      <c r="C55" s="13" t="s">
+    <row r="56" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="12"/>
+      <c r="B56" s="12"/>
+      <c r="C56" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="D55" s="13"/>
-      <c r="E55" s="13" t="s">
+      <c r="D56" s="12"/>
+      <c r="E56" s="12" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="56" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="13"/>
-      <c r="B56" s="13"/>
-      <c r="C56" s="13" t="s">
+    <row r="57" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="12"/>
+      <c r="B57" s="12"/>
+      <c r="C57" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="D56" s="13"/>
-      <c r="E56" s="13" t="s">
+      <c r="D57" s="12"/>
+      <c r="E57" s="12" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="57" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="13"/>
-      <c r="B57" s="13"/>
-      <c r="C57" s="13" t="s">
+    <row r="58" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="12"/>
+      <c r="B58" s="12"/>
+      <c r="C58" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="D57" s="13"/>
-      <c r="E57" s="13" t="s">
+      <c r="D58" s="12"/>
+      <c r="E58" s="12" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="58" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="13"/>
-      <c r="B58" s="13"/>
-      <c r="C58" s="13" t="s">
+    <row r="59" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="12"/>
+      <c r="B59" s="12"/>
+      <c r="C59" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="D58" s="13"/>
-      <c r="E58" s="13" t="s">
+      <c r="D59" s="12"/>
+      <c r="E59" s="12" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="59" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="13"/>
-      <c r="B59" s="13"/>
-      <c r="C59" s="13" t="s">
+    <row r="60" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="12"/>
+      <c r="B60" s="12"/>
+      <c r="C60" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="D59" s="13"/>
-      <c r="E59" s="13" t="s">
+      <c r="D60" s="12"/>
+      <c r="E60" s="12" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="60" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="13"/>
-      <c r="B60" s="13"/>
-      <c r="C60" s="13" t="s">
+    <row r="61" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="12"/>
+      <c r="B61" s="12"/>
+      <c r="C61" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="D60" s="13"/>
-      <c r="E60" s="13" t="s">
+      <c r="D61" s="12"/>
+      <c r="E61" s="12"/>
+    </row>
+    <row r="62" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="12"/>
+      <c r="B62" s="12"/>
+      <c r="C62" s="12" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="13"/>
-      <c r="B61" s="13"/>
-      <c r="C61" s="13" t="s">
+      <c r="D62" s="12"/>
+      <c r="E62" s="12"/>
+    </row>
+    <row r="63" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="12"/>
+      <c r="B63" s="12"/>
+      <c r="C63" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="D61" s="13"/>
-      <c r="E61" s="13"/>
-    </row>
-    <row r="62" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="13"/>
-      <c r="B62" s="13"/>
-      <c r="C62" s="13" t="s">
+      <c r="D63" s="12"/>
+      <c r="E63" s="12"/>
+    </row>
+    <row r="64" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="12"/>
+      <c r="B64" s="12"/>
+      <c r="C64" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="D62" s="13"/>
-      <c r="E62" s="13"/>
-    </row>
-    <row r="63" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="13"/>
-      <c r="B63" s="13"/>
-      <c r="C63" s="13" t="s">
+      <c r="D64" s="12"/>
+      <c r="E64" s="12"/>
+    </row>
+    <row r="65" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="12"/>
+      <c r="B65" s="12"/>
+      <c r="C65" s="12"/>
+      <c r="D65" s="12"/>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="D63" s="13"/>
-      <c r="E63" s="13"/>
-    </row>
-    <row r="64" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="13"/>
-      <c r="B64" s="13"/>
-      <c r="C64" s="13" t="s">
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" s="11" t="s">
         <v>90</v>
-      </c>
-      <c r="D64" s="13"/>
-      <c r="E64" s="13"/>
-    </row>
-    <row r="65" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="13"/>
-      <c r="B65" s="13"/>
-      <c r="C65" s="13"/>
-      <c r="D65" s="13"/>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="12" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="12" t="s">
-        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -1812,119 +1812,119 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="9" width="21.5703125" style="10" customWidth="1"/>
+    <col min="1" max="9" width="21.5703125" style="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
+        <v>91</v>
+      </c>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
     </row>
     <row r="2" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C2" s="16"/>
       <c r="D2" s="17"/>
-      <c r="E2" s="13"/>
+      <c r="E2" s="12"/>
       <c r="F2" s="5"/>
       <c r="G2" s="18" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H2" s="21"/>
     </row>
     <row r="3" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C3" s="16"/>
       <c r="D3" s="17"/>
-      <c r="E3" s="13"/>
+      <c r="E3" s="12"/>
       <c r="F3" s="7"/>
       <c r="G3" s="18" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="H3" s="21"/>
     </row>
     <row r="4" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C4" s="16"/>
       <c r="D4" s="17"/>
-      <c r="E4" s="13"/>
+      <c r="E4" s="12"/>
       <c r="F4" s="4"/>
       <c r="G4" s="18" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H4" s="21"/>
     </row>
     <row r="5" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
-        <v>100</v>
+      <c r="A5" s="10" t="s">
+        <v>98</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C5" s="16"/>
       <c r="D5" s="17"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
     </row>
     <row r="6" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C6" s="16"/>
       <c r="D6" s="17"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12"/>
     </row>
     <row r="7" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C7" s="16"/>
       <c r="D7" s="17"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
     </row>
     <row r="8" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="13"/>
-      <c r="B8" s="13"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
+      <c r="A8" s="12"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
     </row>
     <row r="9" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="22" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B9" s="23"/>
       <c r="C9" s="23"/>
@@ -1933,22 +1933,22 @@
     </row>
     <row r="10" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="C10" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="D10" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="E10" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="F10" s="4" t="s">
         <v>102</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2012,13 +2012,13 @@
       </c>
     </row>
     <row r="14" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="13"/>
-      <c r="B14" s="13"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
+      <c r="A14" s="12"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
     </row>
     <row r="15" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="16" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2048,269 +2048,269 @@
   <dimension ref="A1:N22"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="50" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="B2" sqref="B2:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="14" width="21.5703125" style="10" customWidth="1"/>
+    <col min="1" max="14" width="21.5703125" style="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
+        <v>105</v>
+      </c>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
     </row>
     <row r="2" spans="1:12" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C2" s="16"/>
       <c r="D2" s="17"/>
-      <c r="E2" s="13"/>
+      <c r="E2" s="12"/>
       <c r="F2" s="5"/>
       <c r="G2" s="18" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H2" s="21"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
-      <c r="K2" s="13"/>
-      <c r="L2" s="13"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="12"/>
     </row>
     <row r="3" spans="1:12" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C3" s="16"/>
       <c r="D3" s="17"/>
-      <c r="E3" s="13"/>
+      <c r="E3" s="12"/>
       <c r="F3" s="7"/>
       <c r="G3" s="18" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="H3" s="21"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="13"/>
-      <c r="K3" s="13"/>
-      <c r="L3" s="13"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="12"/>
+      <c r="L3" s="12"/>
     </row>
     <row r="4" spans="1:12" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C4" s="16"/>
       <c r="D4" s="17"/>
-      <c r="E4" s="13"/>
+      <c r="E4" s="12"/>
       <c r="F4" s="4"/>
       <c r="G4" s="18" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H4" s="21"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="13"/>
-      <c r="K4" s="13"/>
-      <c r="L4" s="13"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="12"/>
+      <c r="L4" s="12"/>
     </row>
     <row r="5" spans="1:12" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C5" s="16"/>
       <c r="D5" s="17"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="13"/>
-      <c r="K5" s="13"/>
-      <c r="L5" s="13"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="12"/>
+      <c r="L5" s="12"/>
     </row>
     <row r="6" spans="1:12" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C6" s="16"/>
       <c r="D6" s="17"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="13"/>
-      <c r="I6" s="13"/>
-      <c r="J6" s="13"/>
-      <c r="K6" s="13"/>
-      <c r="L6" s="13"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="12"/>
+      <c r="J6" s="12"/>
+      <c r="K6" s="12"/>
+      <c r="L6" s="12"/>
     </row>
     <row r="7" spans="1:12" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C7" s="16"/>
       <c r="D7" s="17"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13"/>
-      <c r="I7" s="13"/>
-      <c r="J7" s="13"/>
-      <c r="K7" s="13"/>
-      <c r="L7" s="13"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="12"/>
+      <c r="K7" s="12"/>
+      <c r="L7" s="12"/>
     </row>
     <row r="8" spans="1:12" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C8" s="16"/>
       <c r="D8" s="17"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="13"/>
-      <c r="I8" s="13"/>
-      <c r="J8" s="13"/>
-      <c r="K8" s="13"/>
-      <c r="L8" s="13"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="12"/>
+      <c r="K8" s="12"/>
+      <c r="L8" s="12"/>
     </row>
     <row r="9" spans="1:12" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C9" s="16"/>
       <c r="D9" s="17"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="13"/>
-      <c r="I9" s="13"/>
-      <c r="J9" s="13"/>
-      <c r="K9" s="13"/>
-      <c r="L9" s="13"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="12"/>
+      <c r="K9" s="12"/>
+      <c r="L9" s="12"/>
     </row>
     <row r="10" spans="1:12" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C10" s="16"/>
       <c r="D10" s="17"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13"/>
-      <c r="J10" s="13"/>
-      <c r="K10" s="13"/>
-      <c r="L10" s="13"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="12"/>
+      <c r="K10" s="12"/>
+      <c r="L10" s="12"/>
     </row>
     <row r="11" spans="1:12" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C11" s="16"/>
       <c r="D11" s="17"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="13"/>
-      <c r="I11" s="13"/>
-      <c r="J11" s="13"/>
-      <c r="K11" s="13"/>
-      <c r="L11" s="13"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="12"/>
+      <c r="L11" s="12"/>
     </row>
     <row r="12" spans="1:12" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C12" s="16"/>
       <c r="D12" s="17"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="13"/>
-      <c r="I12" s="13"/>
-      <c r="J12" s="13"/>
-      <c r="K12" s="13"/>
-      <c r="L12" s="13"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="12"/>
+      <c r="K12" s="12"/>
+      <c r="L12" s="12"/>
     </row>
     <row r="13" spans="1:12" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C13" s="16"/>
       <c r="D13" s="17"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="13"/>
-      <c r="I13" s="13"/>
-      <c r="J13" s="13"/>
-      <c r="K13" s="13"/>
-      <c r="L13" s="13"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="12"/>
+      <c r="J13" s="12"/>
+      <c r="K13" s="12"/>
+      <c r="L13" s="12"/>
     </row>
     <row r="14" spans="1:12" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="13"/>
-      <c r="B14" s="13"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="13"/>
-      <c r="I14" s="13"/>
-      <c r="J14" s="13"/>
-      <c r="K14" s="13"/>
-      <c r="L14" s="13"/>
+      <c r="A14" s="12"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="12"/>
+      <c r="J14" s="12"/>
+      <c r="K14" s="12"/>
+      <c r="L14" s="12"/>
     </row>
     <row r="15" spans="1:12" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="22" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B15" s="23"/>
       <c r="C15" s="23"/>
@@ -2326,40 +2326,40 @@
     </row>
     <row r="16" spans="1:12" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="B16" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="C16" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="D16" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="E16" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="F16" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="G16" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="F16" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="G16" s="4" t="s">
+      <c r="H16" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="H16" s="4" t="s">
+      <c r="I16" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="I16" s="4" t="s">
+      <c r="J16" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="J16" s="4" t="s">
+      <c r="K16" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="K16" s="4" t="s">
-        <v>126</v>
-      </c>
       <c r="L16" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2477,18 +2477,18 @@
       </c>
     </row>
     <row r="20" spans="1:12" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="13"/>
-      <c r="B20" s="13"/>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
-      <c r="H20" s="13"/>
-      <c r="I20" s="13"/>
-      <c r="J20" s="13"/>
-      <c r="K20" s="13"/>
-      <c r="L20" s="13"/>
+      <c r="A20" s="12"/>
+      <c r="B20" s="12"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="12"/>
+      <c r="J20" s="12"/>
+      <c r="K20" s="12"/>
+      <c r="L20" s="12"/>
     </row>
     <row r="21" spans="1:12" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="22" spans="1:12" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>